<commit_message>
Compound equivalents in entry 6 updated
</commit_message>
<xml_diff>
--- a/Code_And_Data/Dataset/TestingData.xlsx
+++ b/Code_And_Data/Dataset/TestingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/upasanaroy/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/upasanaroy/Documents/AI_Chem_Github/Yield-Prediction/Code_And_Data/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F361212-6D1B-BC41-8A9E-911CF384579B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503CA96A-6956-D747-8250-A12D68C3312F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,9 +197,6 @@
     <t>Toluene</t>
   </si>
   <si>
-    <t>Benzenamine hydrochloride (1:1)</t>
-  </si>
-  <si>
     <t>Tetrahydrofuran:Water</t>
   </si>
   <si>
@@ -332,6 +329,9 @@
   </si>
   <si>
     <t>Reaction_Yield</t>
+  </si>
+  <si>
+    <t>Benzenamine hydrochloride</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1037,13 +1037,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1070,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N1" s="10" t="s">
         <v>10</v>
@@ -1257,28 +1257,28 @@
         <v>38</v>
       </c>
       <c r="B6" s="11">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="D6" s="20">
         <v>1</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="21">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>49</v>
       </c>
       <c r="H6" s="11">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J6" s="21">
         <v>0.01</v>
@@ -1293,7 +1293,7 @@
         <v>100</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="20">
@@ -1304,13 +1304,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="20">
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="21">
         <v>1</v>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="21">
         <v>0.625</v>
@@ -1337,30 +1337,30 @@
         <v>68</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="22">
       <c r="A8" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="27">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="28" t="s">
+      <c r="D8" s="29">
+        <v>1</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>65</v>
-      </c>
-      <c r="D8" s="29">
-        <v>1</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>66</v>
       </c>
       <c r="F8" s="31">
         <v>1.23</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="31">
         <v>2.52</v>
@@ -1381,30 +1381,30 @@
         <v>84</v>
       </c>
       <c r="N8" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="22">
       <c r="A9" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="27">
         <v>1</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="29">
         <v>1</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="31">
         <v>1.23</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" s="31">
         <v>2.52</v>
@@ -1425,7 +1425,7 @@
         <v>92</v>
       </c>
       <c r="N9" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="22">
@@ -1436,19 +1436,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="29">
         <v>1</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="31">
         <v>1.23</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="31">
         <v>2.52</v>
@@ -1469,30 +1469,30 @@
         <v>82</v>
       </c>
       <c r="N10" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="22">
       <c r="A11" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="27">
         <v>1</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="29">
         <v>1</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="31">
         <v>1.23</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="31">
         <v>2.52</v>
@@ -1513,36 +1513,36 @@
         <v>63</v>
       </c>
       <c r="N11" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20">
       <c r="A12" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="27">
         <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="29">
+        <v>1</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>72</v>
-      </c>
-      <c r="D12" s="29">
-        <v>1</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>73</v>
       </c>
       <c r="F12" s="31">
         <v>1.1000000000000001</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12" s="31">
         <v>3.1</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" s="31">
         <v>0.5</v>
@@ -1557,7 +1557,7 @@
         <v>97</v>
       </c>
       <c r="N12" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20">
@@ -1794,7 +1794,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="35">
         <v>1.25</v>
@@ -1865,18 +1865,18 @@
         <v>54</v>
       </c>
       <c r="N19" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="22">
       <c r="A20" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="42">
         <v>1</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" s="35">
         <v>1</v>
@@ -1888,13 +1888,13 @@
         <v>1.3</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20" s="42">
         <v>2</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J20" s="42">
         <v>0.5</v>
@@ -1909,7 +1909,7 @@
         <v>84</v>
       </c>
       <c r="N20" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="22">
@@ -1920,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="35">
         <v>1</v>
@@ -1932,13 +1932,13 @@
         <v>1.3</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="42">
         <v>2</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" s="42">
         <v>0.5</v>
@@ -1953,7 +1953,7 @@
         <v>93</v>
       </c>
       <c r="N21" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1973,6 +1973,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="f006263b-6855-4f81-be49-4241caee7f23">
@@ -1983,7 +1992,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBC1E36CE2333A4DBCA9CD5063464EF8" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9620bf27d4ff32933b9f2337e2be106">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f006263b-6855-4f81-be49-4241caee7f23" xmlns:ns3="dabe3c20-206e-48c2-bf8d-a29783c980eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d08129629143736746fb52b30a130668" ns2:_="" ns3:_="">
     <xsd:import namespace="f006263b-6855-4f81-be49-4241caee7f23"/>
@@ -2206,27 +2215,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C683F71-BAD6-45A7-9C46-62C2D2F63BFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65EBFEDB-1F62-4F1C-B496-B4021A8B8AE1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f006263b-6855-4f81-be49-4241caee7f23"/>
-    <ds:schemaRef ds:uri="dabe3c20-206e-48c2-bf8d-a29783c980eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C683F71-BAD6-45A7-9C46-62C2D2F63BFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f006263b-6855-4f81-be49-4241caee7f23"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dabe3c20-206e-48c2-bf8d-a29783c980eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB92CAC3-9F74-4995-820F-13C750327611}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2243,12 +2257,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65EBFEDB-1F62-4F1C-B496-B4021A8B8AE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>